<commit_message>
Added new TC B005 & updated testdata.xlsx
</commit_message>
<xml_diff>
--- a/Flipkart/testdata/testdata.xlsx
+++ b/Flipkart/testdata/testdata.xlsx
@@ -1,24 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{30FD9185-27CA-489D-830F-47407BD09708}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Bala/git/Flipkart/Flipkart/testdata/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17005720-16F0-3D40-BFF8-ECBE74B8123D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30" yWindow="630" windowWidth="14865" windowHeight="9900" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="40" yWindow="640" windowWidth="14860" windowHeight="9900" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TC002" sheetId="1" r:id="rId1"/>
     <sheet name="TC003" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="TC004" sheetId="4" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:K4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="13">
   <si>
     <t>Dresses</t>
   </si>
@@ -452,9 +457,9 @@
       <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -468,7 +473,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -491,13 +496,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -511,7 +516,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -525,7 +530,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -539,7 +544,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -553,7 +558,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -567,7 +572,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -588,12 +593,61 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2058BD4-0018-9240-8535-D17C6EBB03A5}">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D4" s="2"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D5" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>